<commit_message>
docs(fase1): atualiza relatorio excel com paineis visuais e graficos do powerpoint
</commit_message>
<xml_diff>
--- a/fase1-simulacao-calculadora-aws/relatorio_sap.xlsx
+++ b/fase1-simulacao-calculadora-aws/relatorio_sap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aldec\Downloads\TheCloudBootecamp\modulo-6\sap-migration-to-aws\fase1-simulacao-calculadora-aws\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5DE00E7B-9CC7-4BC5-AB34-DF75E07F13DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{748600AA-F061-49D2-BD50-18C396F6138B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t>Environment</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>91.501,56</t>
+  </si>
+  <si>
+    <t>15,000.00</t>
   </si>
 </sst>
 </file>
@@ -531,6 +534,111 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>112058</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6353</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>145676</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>8032</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B793D31C-CC43-8952-6A69-193032DB75D7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8247529" y="6353"/>
+          <a:ext cx="8983943" cy="3030442"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>116914</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>134470</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>88152</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{261F5B48-5310-64EE-7CFA-FF061855F2D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8252385" y="3092823"/>
+          <a:ext cx="8971056" cy="3334683"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -821,7 +929,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -987,8 +1095,8 @@
       <c r="C9" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="25">
-        <v>15000</v>
+      <c r="D9" s="25" t="s">
+        <v>71</v>
       </c>
       <c r="E9" s="33">
         <v>180000</v>
@@ -1211,19 +1319,19 @@
       <c r="E28" s="30"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
+      <c r="A29" s="8"/>
+      <c r="B29" s="28"/>
+      <c r="C29" s="13"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="30"/>
       <c r="F29" s="5"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="13"/>
+      <c r="D30" s="8"/>
+      <c r="E30" s="30"/>
       <c r="F30" s="5"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1260,6 +1368,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>